<commit_message>
Code Optimization  (24 Feb 2023)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\603214\Documents\UiPath\Global Foundries Process\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F09ABF-B425-4473-8873-CF1D066CB9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00360BF-82A7-489D-8A10-BC06ED704DAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t>00:00:03</t>
+  </si>
+  <si>
+    <t>ShareDrive_DownloadedFlatFileFolderPath</t>
+  </si>
+  <si>
+    <t>GF_ShareDriveDownloadedFlatFileFolderPath</t>
   </si>
 </sst>
 </file>
@@ -1746,7 +1752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -2972,8 +2978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3020,7 +3026,14 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>